<commit_message>
Commit 10: criado a view com o detalhe dos atrasos no relatório
</commit_message>
<xml_diff>
--- a/Teste/teste_alunos2.xlsx
+++ b/Teste/teste_alunos2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2947685926b3e492/Documentos/GitHub/UNIVESP-PI-Sistema_Gerenciador_de_Atrasos/Teste/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9E1B8C18-654C-4898-98C4-BD658677F0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC9450AD-83D4-412E-8ADA-2C0D79DE969B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{9E1B8C18-654C-4898-98C4-BD658677F0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3845EB59-9459-4516-AB6B-022ECEF86B99}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{077E4775-C7D5-400F-B51C-35EADCF32792}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>R.A.</t>
   </si>
@@ -167,13 +167,25 @@
   </si>
   <si>
     <t>Responsável 2</t>
+  </si>
+  <si>
+    <t>Aluno 21</t>
+  </si>
+  <si>
+    <t>Rua do Aluno 21</t>
+  </si>
+  <si>
+    <t>Pai do Aluno 21</t>
+  </si>
+  <si>
+    <t>Mãe do Aluno 21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +316,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -708,6 +726,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1027,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8E3125-0512-415E-8725-BC38948E20FC}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A9" sqref="A9:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1297,7 +1319,31 @@
         <v>11987654340</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>202521</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12">
+        <v>11987654341</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>